<commit_message>
Act. se determino la zona horaria del sistema en general, se agrego el modulo de cotizaciones y venta mediante factura
</commit_message>
<xml_diff>
--- a/archivos/Inventario_Productos.xlsx
+++ b/archivos/Inventario_Productos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\dist_guadalupana\archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96F35BA-0D26-4E10-B710-1B1B58D8FBE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D313873D-3603-4628-AECD-49D421F6C783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Productos" sheetId="1" r:id="rId1"/>
@@ -4041,7 +4041,7 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -4300,8 +4300,8 @@
   <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4337,7 +4337,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B2" s="22" t="s">
         <v>42</v>
@@ -4348,7 +4348,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="11">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>17</v>

</xml_diff>